<commit_message>
Add batch upload by Excel templates
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/Library/CloudStorage/Dropbox/My Mac (10-17-233-196.dynapool.wireless.nyu.edu)/Desktop/splitgal4.org/splitgal4db/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645B0D65-A30A-6D48-8666-43361D829E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A963ECB7-3241-1C45-92ED-7244A857EDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
+    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
   </bookViews>
   <sheets>
     <sheet name="List of lines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Gene name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Private</t>
   </si>
   <si>
-    <t>Validated</t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
@@ -202,6 +199,15 @@
   </si>
   <si>
     <t>This is an example. Please remove it before you upload.</t>
+  </si>
+  <si>
+    <t>MI99999</t>
+  </si>
+  <si>
+    <t>Available (Validated)</t>
+  </si>
+  <si>
+    <t>Available (Not validated)</t>
   </si>
 </sst>
 </file>
@@ -575,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64B5C7-850F-C748-A8B5-75882E5545E8}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +611,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -620,12 +626,12 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -637,28 +643,31 @@
         <v>6667842</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
       <c r="D3" t="s">
         <v>20</v>
       </c>
@@ -666,19 +675,19 @@
         <v>6732753</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -738,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86360827-EA7E-4647-A275-CC2BA72C92E0}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,7 +780,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -803,7 +812,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
@@ -823,13 +832,13 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -843,13 +852,13 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
         <v>30</v>
@@ -863,10 +872,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -877,7 +886,7 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update field value and display
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/Library/CloudStorage/Dropbox/My Mac (10-17-233-196.dynapool.wireless.nyu.edu)/Desktop/splitgal4.org/splitgal4db/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A963ECB7-3241-1C45-92ED-7244A857EDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EFE0EA-8656-DB43-8262-F49173D6CF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
+    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
   </bookViews>
   <sheets>
     <sheet name="List of lines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>Gene name</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>In progress</t>
-  </si>
-  <si>
-    <t>Available</t>
   </si>
   <si>
     <t>Planned</t>
@@ -581,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64B5C7-850F-C748-A8B5-75882E5545E8}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -611,7 +608,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -626,12 +623,12 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -643,30 +640,30 @@
         <v>6667842</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
         <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
         <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
         <v>20</v>
@@ -675,19 +672,19 @@
         <v>6732753</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -747,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86360827-EA7E-4647-A275-CC2BA72C92E0}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -780,7 +777,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -812,7 +809,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>25</v>
@@ -832,13 +829,13 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
         <v>24</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -852,7 +849,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
@@ -872,10 +869,10 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -886,7 +883,7 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Refactor to make database structure template-based
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/Library/CloudStorage/Dropbox/My Mac (10-17-233-196.dynapool.wireless.nyu.edu)/Desktop/splitgal4.org/splitgal4db/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/OrbStack/docker/volumes/2f475c6a891f421c7e0bdc58789dd193c90e096cc47b8e9d5fb602a3609bd5cd/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7914B85C-468C-1447-B2D0-F93C68EDD959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F328633-D77D-5E4F-8C33-09DFE26E4DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
+    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
   </bookViews>
   <sheets>
     <sheet name="List of lines" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t>Gene name</t>
   </si>
@@ -205,6 +205,30 @@
   </si>
   <si>
     <t>Other ADs</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t>Please leave blank if your lab generated this line. If you obtained this line from other researchers, please leave their name here.</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>If left blank, the contact information from your account will be used. If you want people to request via a different mail, or if the line is from another lab and you know their preferred mail, please leave that here.</t>
+  </si>
+  <si>
+    <t>Cassette style</t>
+  </si>
+  <si>
+    <t>Dimerization Domain</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Citation</t>
   </si>
 </sst>
 </file>
@@ -576,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64B5C7-850F-C748-A8B5-75882E5545E8}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,10 +612,10 @@
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="11" max="11" width="37.5" customWidth="1"/>
+    <col min="13" max="13" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,25 +632,31 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -651,11 +681,11 @@
       <c r="I2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -683,15 +713,16 @@
       <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{658651A3-530E-C046-911F-2F75DDCC5DD8}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="G1 H1 I1" xr:uid="{0B5F877C-F749-914E-9B83-E58690E95252}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -704,35 +735,35 @@
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C06905ED-A3C7-794E-ABC1-3948642869EA}">
-          <x14:formula1>
-            <xm:f>Instruction!$G$3:$G$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CFE71482-7501-924E-A31D-954B78523E8A}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{CFE71482-7501-924E-A31D-954B78523E8A}">
           <x14:formula1>
             <xm:f>Instruction!$I$3:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{775E4C98-E28F-A247-BB8F-64F5E241545D}">
           <x14:formula1>
             <xm:f>Instruction!$F$3:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{44ABAAC1-7306-9947-9BF9-536181DB0595}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{44ABAAC1-7306-9947-9BF9-536181DB0595}">
           <x14:formula1>
             <xm:f>Instruction!$H$3:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16F77697-3CCF-7E46-95A8-894763B6461A}">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{16F77697-3CCF-7E46-95A8-894763B6461A}">
           <x14:formula1>
             <xm:f>Instruction!$B$3:$B$8</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1BEFAA88-5296-1142-AAE6-CF88DFE7F9CE}">
+          <x14:formula1>
+            <xm:f>Instruction!$G$3:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -742,10 +773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86360827-EA7E-4647-A275-CC2BA72C92E0}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,10 +788,10 @@
     <col min="5" max="6" width="30.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="9" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -789,10 +820,16 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -820,8 +857,14 @@
       <c r="I2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -841,7 +884,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -861,7 +904,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -875,7 +918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -883,7 +926,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>43</v>
       </c>
@@ -891,7 +934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Couple the database with the template
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/OrbStack/docker/volumes/2f475c6a891f421c7e0bdc58789dd193c90e096cc47b8e9d5fb602a3609bd5cd/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ycc/OrbStack/docker/volumes/b93966e6ac1b67af07e0f9ed167846e3570ff185bee62024ebef19a13a7c694e/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F328633-D77D-5E4F-8C33-09DFE26E4DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70BF035-EE19-3247-AA44-9E95A30333F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17720" yWindow="1800" windowWidth="27240" windowHeight="16440" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
+    <workbookView xWindow="51200" yWindow="-4560" windowWidth="21600" windowHeight="37900" activeTab="1" xr2:uid="{B20FDCF2-ECA3-7748-8913-1CAB62C760D7}"/>
   </bookViews>
   <sheets>
     <sheet name="List of lines" sheetId="2" r:id="rId1"/>
@@ -37,24 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Gene name</t>
   </si>
   <si>
     <t>MiMIC/CRIMIC #</t>
-  </si>
-  <si>
-    <t>Effectors</t>
-  </si>
-  <si>
-    <t>chromosome</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
-    <t>dimerization domain</t>
   </si>
   <si>
     <t>citation</t>
@@ -174,9 +162,6 @@
     <t>pb</t>
   </si>
   <si>
-    <t>cassette style</t>
-  </si>
-  <si>
     <t>What type of cassette is used for the effector?</t>
   </si>
   <si>
@@ -207,28 +192,67 @@
     <t>Other ADs</t>
   </si>
   <si>
+    <t>gene_name</t>
+  </si>
+  <si>
+    <t>effector_type</t>
+  </si>
+  <si>
+    <t>source_id</t>
+  </si>
+  <si>
+    <t>cassette</t>
+  </si>
+  <si>
+    <t>ins_seqname</t>
+  </si>
+  <si>
+    <t>ins_site</t>
+  </si>
+  <si>
+    <t>dimerizer</t>
+  </si>
+  <si>
+    <t>contributor</t>
+  </si>
+  <si>
+    <t>Please provide the source lab if the line is not generated from your lab</t>
+  </si>
+  <si>
+    <t>Effector</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Cassette</t>
+  </si>
+  <si>
+    <t>Dimerization domain</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>Contributor</t>
   </si>
   <si>
-    <t>Please leave blank if your lab generated this line. If you obtained this line from other researchers, please leave their name here.</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>If left blank, the contact information from your account will be used. If you want people to request via a different mail, or if the line is from another lab and you know their preferred mail, please leave that here.</t>
-  </si>
-  <si>
-    <t>Cassette style</t>
-  </si>
-  <si>
-    <t>Dimerization Domain</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Citation</t>
+  </si>
+  <si>
+    <t>Citation info for the line (PMID is preferred)</t>
+  </si>
+  <si>
+    <t>Other notes that you want to share with others</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -600,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C64B5C7-850F-C748-A8B5-75882E5545E8}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,117 +636,113 @@
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="6" width="16.5" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="13" max="13" width="37.5" customWidth="1"/>
+    <col min="12" max="12" width="37.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D1" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>6667842</v>
       </c>
       <c r="F2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>6732753</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{658651A3-530E-C046-911F-2F75DDCC5DD8}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="G1 H1 I1" xr:uid="{0B5F877C-F749-914E-9B83-E58690E95252}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -731,39 +751,39 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F04ED5F8-8657-AE49-AD4B-78AF2F857652}">
           <x14:formula1>
-            <xm:f>Instruction!$D$3:$D$8</xm:f>
+            <xm:f>Instruction!$D$4:$D$9</xm:f>
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{CFE71482-7501-924E-A31D-954B78523E8A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C06905ED-A3C7-794E-ABC1-3948642869EA}">
           <x14:formula1>
-            <xm:f>Instruction!$I$3:$I$4</xm:f>
+            <xm:f>Instruction!$G$4:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CFE71482-7501-924E-A31D-954B78523E8A}">
+          <x14:formula1>
+            <xm:f>Instruction!$I$4:$I$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{775E4C98-E28F-A247-BB8F-64F5E241545D}">
           <x14:formula1>
-            <xm:f>Instruction!$F$3:$F$5</xm:f>
+            <xm:f>Instruction!$F$4:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{44ABAAC1-7306-9947-9BF9-536181DB0595}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{44ABAAC1-7306-9947-9BF9-536181DB0595}">
           <x14:formula1>
-            <xm:f>Instruction!$H$3:$H$5</xm:f>
+            <xm:f>Instruction!$H$4:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{16F77697-3CCF-7E46-95A8-894763B6461A}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16F77697-3CCF-7E46-95A8-894763B6461A}">
           <x14:formula1>
-            <xm:f>Instruction!$B$3:$B$8</xm:f>
+            <xm:f>Instruction!$B$4:$B$9</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1BEFAA88-5296-1142-AAE6-CF88DFE7F9CE}">
-          <x14:formula1>
-            <xm:f>Instruction!$G$3:$G$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -773,10 +793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86360827-EA7E-4647-A275-CC2BA72C92E0}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +808,9 @@
     <col min="5" max="6" width="30.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="11" width="25" customWidth="1"/>
+    <col min="9" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -796,153 +818,195 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="59" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="136" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
+      <c r="K3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="2">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>